<commit_message>
No revisar aún. No entres. No abras. No leas. Que aún no está listo... :)
</commit_message>
<xml_diff>
--- a/2014/EVOStar/Co-Genebot (EVOGames)/Estudios/CoGene-PrimerasComparativas.xlsx
+++ b/2014/EVOStar/Co-Genebot (EVOGames)/Estudios/CoGene-PrimerasComparativas.xlsx
@@ -1041,11 +1041,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="139555968"/>
-        <c:axId val="139557504"/>
+        <c:axId val="208939648"/>
+        <c:axId val="208961920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139555968"/>
+        <c:axId val="208939648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1054,12 +1054,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139557504"/>
+        <c:crossAx val="208961920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139557504"/>
+        <c:axId val="208961920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1070,7 +1070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139555968"/>
+        <c:crossAx val="208939648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4636,11 +4636,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140509184"/>
-        <c:axId val="140510720"/>
+        <c:axId val="210228736"/>
+        <c:axId val="210230272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140509184"/>
+        <c:axId val="210228736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4649,7 +4649,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140510720"/>
+        <c:crossAx val="210230272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4657,7 +4657,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140510720"/>
+        <c:axId val="210230272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4668,14 +4668,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140509184"/>
+        <c:crossAx val="210228736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7812,11 +7811,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140546048"/>
-        <c:axId val="140547584"/>
+        <c:axId val="210003456"/>
+        <c:axId val="210004992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140546048"/>
+        <c:axId val="210003456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7825,7 +7824,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140547584"/>
+        <c:crossAx val="210004992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7833,7 +7832,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140547584"/>
+        <c:axId val="210004992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7844,7 +7843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140546048"/>
+        <c:crossAx val="210003456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11110,11 +11109,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140681216"/>
-        <c:axId val="140682752"/>
+        <c:axId val="210096896"/>
+        <c:axId val="210098816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140681216"/>
+        <c:axId val="210096896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11142,7 +11141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140682752"/>
+        <c:crossAx val="210098816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11152,7 +11151,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140682752"/>
+        <c:axId val="210098816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -11188,7 +11187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140681216"/>
+        <c:crossAx val="210096896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12115,11 +12114,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="139721344"/>
-        <c:axId val="139989376"/>
+        <c:axId val="209109376"/>
+        <c:axId val="209110912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139721344"/>
+        <c:axId val="209109376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12128,12 +12127,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139989376"/>
+        <c:crossAx val="209110912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139989376"/>
+        <c:axId val="209110912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12144,14 +12143,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139721344"/>
+        <c:crossAx val="209109376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15499,11 +15497,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139734016"/>
-        <c:axId val="139744000"/>
+        <c:axId val="209134336"/>
+        <c:axId val="209135872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139734016"/>
+        <c:axId val="209134336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15512,7 +15510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139744000"/>
+        <c:crossAx val="209135872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15520,7 +15518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139744000"/>
+        <c:axId val="209135872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15531,7 +15529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139734016"/>
+        <c:crossAx val="209134336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18885,11 +18883,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139874688"/>
-        <c:axId val="139876224"/>
+        <c:axId val="209273216"/>
+        <c:axId val="209274752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139874688"/>
+        <c:axId val="209273216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18898,7 +18896,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139876224"/>
+        <c:crossAx val="209274752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18906,7 +18904,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139876224"/>
+        <c:axId val="209274752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18917,14 +18915,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139874688"/>
+        <c:crossAx val="209273216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -18964,7 +18961,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -19031,7 +19027,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -19076,7 +19071,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -19143,7 +19137,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -22460,11 +22453,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140374016"/>
-        <c:axId val="140375552"/>
+        <c:axId val="209798656"/>
+        <c:axId val="209800192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140374016"/>
+        <c:axId val="209798656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22473,7 +22466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140375552"/>
+        <c:crossAx val="209800192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22481,7 +22474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140375552"/>
+        <c:axId val="209800192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22492,14 +22485,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140374016"/>
+        <c:crossAx val="209798656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -25816,11 +25808,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140386304"/>
-        <c:axId val="140387840"/>
+        <c:axId val="209585664"/>
+        <c:axId val="209587200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140386304"/>
+        <c:axId val="209585664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25829,7 +25821,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140387840"/>
+        <c:crossAx val="209587200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25837,7 +25829,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140387840"/>
+        <c:axId val="209587200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25848,14 +25840,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140386304"/>
+        <c:crossAx val="209585664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -29172,11 +29163,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="140427264"/>
-        <c:axId val="140428800"/>
+        <c:axId val="209647104"/>
+        <c:axId val="209648640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140427264"/>
+        <c:axId val="209647104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29185,7 +29176,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140428800"/>
+        <c:crossAx val="209648640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -29193,7 +29184,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140428800"/>
+        <c:axId val="209648640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -29204,14 +29195,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140427264"/>
+        <c:crossAx val="209647104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>

</xml_diff>